<commit_message>
change title in product page
</commit_message>
<xml_diff>
--- a/category/Category page.xlsx
+++ b/category/Category page.xlsx
@@ -676,7 +676,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1011,26 +1011,6 @@
         <color rgb="FF464B51"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF464B51"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF464B51"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF464B51"/>
-      </left>
-      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1040,7 +1020,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1261,17 +1241,23 @@
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1321,15 +1307,6 @@
     <xf numFmtId="0" fontId="20" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
     </xf>
@@ -1356,9 +1333,6 @@
     </xf>
     <xf numFmtId="0" fontId="27" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -24284,246 +24258,34 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>38099</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>314324</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>566324</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="465" name="Rounded Rectangle 464"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7258049" y="2505074"/>
-          <a:ext cx="1743076" cy="252000"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF6600"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Deal Of The Day</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>314324</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>333374</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>585374</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="466" name="Rounded Rectangle 465"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8963024" y="2524124"/>
-          <a:ext cx="1743076" cy="252000"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF6600"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Flash</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="FF6600"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> Deal</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-GB" sz="1000" b="1">
-            <a:solidFill>
-              <a:srgbClr val="FF6600"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>323849</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>575849</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="467" name="Rounded Rectangle 466"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10934699" y="2514599"/>
-          <a:ext cx="1743076" cy="252000"/>
-        </a:xfrm>
-        <a:prstGeom prst="roundRect">
-          <a:avLst>
-            <a:gd name="adj" fmla="val 0"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="6350">
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-GB" sz="1000" b="1">
-              <a:solidFill>
-                <a:srgbClr val="FF6600"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>Deal Ending Soon</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>357188</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>1414463</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>421274</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>314326</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>228599</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="470" name="Elbow Connector 469"/>
         <xdr:cNvCxnSpPr>
+          <a:stCxn id="63" idx="0"/>
           <a:endCxn id="5" idx="3"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="11106150" y="1414463"/>
-          <a:ext cx="1390650" cy="1197561"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="5492751" y="88900"/>
+          <a:ext cx="1592261" cy="4243388"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector4">
           <a:avLst>
-            <a:gd name="adj1" fmla="val -16438"/>
+            <a:gd name="adj1" fmla="val 28913"/>
+            <a:gd name="adj2" fmla="val 105387"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -25988,8 +25750,8 @@
   </sheetPr>
   <dimension ref="A1:Z389"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P182" sqref="P182"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="18.75" customHeight="1"/>
@@ -26006,31 +25768,31 @@
   <sheetData>
     <row r="1" spans="1:24" ht="172.5" customHeight="1"/>
     <row r="2" spans="1:24" ht="46.5" customHeight="1">
-      <c r="A2" s="82"/>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
-      <c r="M2" s="83"/>
-      <c r="N2" s="83"/>
-      <c r="O2" s="83"/>
-      <c r="P2" s="83"/>
-      <c r="Q2" s="83"/>
-      <c r="R2" s="83"/>
-      <c r="S2" s="83"/>
-      <c r="T2" s="83"/>
-      <c r="U2" s="83"/>
-      <c r="V2" s="83"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="X2" s="5"/>
     </row>
     <row r="3" spans="1:24" ht="60" customHeight="1">
-      <c r="A3" s="84"/>
+      <c r="A3" s="82"/>
       <c r="B3" s="70"/>
       <c r="C3" s="70"/>
       <c r="D3" s="70"/>
@@ -26054,7 +25816,7 @@
       <c r="V3" s="25"/>
     </row>
     <row r="4" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A4" s="85"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
       <c r="D4" s="71"/>
@@ -26077,33 +25839,33 @@
       <c r="U4" s="71"/>
     </row>
     <row r="5" spans="1:24" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A5" s="85"/>
-      <c r="B5" s="102"/>
-      <c r="C5" s="102"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="102"/>
-      <c r="F5" s="102"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="102"/>
-      <c r="I5" s="102"/>
-      <c r="J5" s="102"/>
-      <c r="K5" s="102"/>
-      <c r="L5" s="102"/>
-      <c r="M5" s="102"/>
-      <c r="N5" s="102"/>
-      <c r="O5" s="102"/>
-      <c r="P5" s="102"/>
+      <c r="A5" s="83"/>
+      <c r="B5" s="87"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="87"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="87"/>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="87"/>
+      <c r="J5" s="87"/>
+      <c r="K5" s="87"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
+      <c r="N5" s="87"/>
+      <c r="O5" s="87"/>
+      <c r="P5" s="87"/>
       <c r="Q5" s="73"/>
-      <c r="R5" s="102"/>
-      <c r="S5" s="102"/>
-      <c r="T5" s="102"/>
-      <c r="U5" s="102"/>
-      <c r="V5" s="114"/>
+      <c r="R5" s="87"/>
+      <c r="S5" s="87"/>
+      <c r="T5" s="87"/>
+      <c r="U5" s="87"/>
+      <c r="V5" s="84"/>
       <c r="W5" s="38"/>
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="85"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
       <c r="D6" s="34"/>
@@ -26112,12 +25874,12 @@
       <c r="G6" s="34"/>
       <c r="H6" s="34"/>
       <c r="I6" s="35"/>
-      <c r="J6" s="96" t="s">
+      <c r="J6" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="97"/>
-      <c r="L6" s="97"/>
-      <c r="M6" s="98"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="100"/>
       <c r="N6" s="31"/>
       <c r="O6" s="32"/>
       <c r="P6" s="32"/>
@@ -26126,12 +25888,12 @@
       <c r="S6" s="33"/>
       <c r="T6" s="33"/>
       <c r="U6" s="33"/>
-      <c r="V6" s="114"/>
+      <c r="V6" s="84"/>
       <c r="W6" s="38"/>
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="1:24" ht="15" customHeight="1" thickBot="1">
-      <c r="A7" s="85"/>
+      <c r="A7" s="83"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -26140,10 +25902,10 @@
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
-      <c r="J7" s="99"/>
-      <c r="K7" s="100"/>
-      <c r="L7" s="100"/>
-      <c r="M7" s="101"/>
+      <c r="J7" s="101"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="103"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -26152,11 +25914,11 @@
       <c r="S7" s="5"/>
       <c r="T7" s="5"/>
       <c r="U7" s="5"/>
-      <c r="V7" s="114"/>
+      <c r="V7" s="84"/>
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A8" s="85"/>
+      <c r="A8" s="83"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -26177,12 +25939,12 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
-      <c r="V8" s="114"/>
+      <c r="V8" s="84"/>
       <c r="W8" s="38"/>
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A9" s="85"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
@@ -26207,7 +25969,7 @@
       <c r="X9" s="2"/>
     </row>
     <row r="10" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A10" s="85"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -26232,7 +25994,7 @@
       <c r="X10" s="2"/>
     </row>
     <row r="11" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A11" s="85"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="72"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -26257,7 +26019,7 @@
       <c r="X11" s="2"/>
     </row>
     <row r="12" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A12" s="85"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -26282,7 +26044,7 @@
       <c r="X12" s="2"/>
     </row>
     <row r="13" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A13" s="85"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -26307,7 +26069,7 @@
       <c r="X13" s="2"/>
     </row>
     <row r="14" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A14" s="85"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -26332,7 +26094,7 @@
       <c r="X14" s="2"/>
     </row>
     <row r="15" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A15" s="85"/>
+      <c r="A15" s="83"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
@@ -26357,7 +26119,7 @@
       <c r="X15" s="2"/>
     </row>
     <row r="16" spans="1:24" ht="18.75" customHeight="1">
-      <c r="A16" s="85"/>
+      <c r="A16" s="83"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -26382,7 +26144,7 @@
       <c r="X16" s="2"/>
     </row>
     <row r="17" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A17" s="85"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -26407,7 +26169,7 @@
       <c r="X17" s="2"/>
     </row>
     <row r="18" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A18" s="85"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -26432,7 +26194,7 @@
       <c r="X18" s="2"/>
     </row>
     <row r="19" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A19" s="85"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -26457,7 +26219,7 @@
       <c r="X19" s="2"/>
     </row>
     <row r="20" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A20" s="85"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -26482,7 +26244,7 @@
       <c r="X20" s="2"/>
     </row>
     <row r="21" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A21" s="85"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -26507,7 +26269,7 @@
       <c r="X21" s="2"/>
     </row>
     <row r="22" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A22" s="85"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -26530,7 +26292,7 @@
       <c r="U22" s="5"/>
     </row>
     <row r="23" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A23" s="85"/>
+      <c r="A23" s="83"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -26553,7 +26315,7 @@
       <c r="U23" s="5"/>
     </row>
     <row r="24" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A24" s="85"/>
+      <c r="A24" s="83"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -26576,7 +26338,7 @@
       <c r="U24" s="5"/>
     </row>
     <row r="25" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A25" s="85"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
@@ -26599,7 +26361,7 @@
       <c r="U25" s="21"/>
     </row>
     <row r="26" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A26" s="85"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -26626,7 +26388,7 @@
       <c r="Z26" s="20"/>
     </row>
     <row r="27" spans="1:26" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A27" s="85"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -26653,19 +26415,19 @@
       <c r="Z27" s="20"/>
     </row>
     <row r="28" spans="1:26" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A28" s="85"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="28"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29"/>
       <c r="E28" s="29"/>
       <c r="F28" s="30"/>
-      <c r="G28" s="90" t="s">
+      <c r="G28" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="H28" s="91"/>
-      <c r="I28" s="91"/>
-      <c r="J28" s="91"/>
-      <c r="K28" s="92"/>
+      <c r="H28" s="93"/>
+      <c r="I28" s="93"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="94"/>
       <c r="L28" s="26"/>
       <c r="M28" s="27"/>
       <c r="N28" s="27"/>
@@ -26673,10 +26435,10 @@
       <c r="P28" s="27"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="36"/>
-      <c r="S28" s="86" t="s">
+      <c r="S28" s="88" t="s">
         <v>61</v>
       </c>
-      <c r="T28" s="87"/>
+      <c r="T28" s="89"/>
       <c r="U28" s="37"/>
       <c r="W28" s="20"/>
       <c r="X28" s="20"/>
@@ -26684,17 +26446,17 @@
       <c r="Z28" s="20"/>
     </row>
     <row r="29" spans="1:26" ht="15" customHeight="1" thickBot="1">
-      <c r="A29" s="85"/>
+      <c r="A29" s="83"/>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="93"/>
-      <c r="H29" s="94"/>
-      <c r="I29" s="94"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="95"/>
+      <c r="G29" s="95"/>
+      <c r="H29" s="96"/>
+      <c r="I29" s="96"/>
+      <c r="J29" s="96"/>
+      <c r="K29" s="97"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
       <c r="N29" s="5"/>
@@ -26702,12 +26464,12 @@
       <c r="P29" s="6"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="23"/>
-      <c r="S29" s="88"/>
-      <c r="T29" s="89"/>
+      <c r="S29" s="90"/>
+      <c r="T29" s="91"/>
       <c r="U29" s="43"/>
     </row>
     <row r="30" spans="1:26" ht="15" customHeight="1">
-      <c r="A30" s="85"/>
+      <c r="A30" s="83"/>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -26730,7 +26492,7 @@
       <c r="U30" s="43"/>
     </row>
     <row r="31" spans="1:26" ht="15" customHeight="1">
-      <c r="A31" s="85"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="72"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -26753,7 +26515,7 @@
       <c r="U31" s="21"/>
     </row>
     <row r="32" spans="1:26" ht="24.75" customHeight="1">
-      <c r="A32" s="85"/>
+      <c r="A32" s="83"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -26776,7 +26538,7 @@
       <c r="U32" s="21"/>
     </row>
     <row r="33" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A33" s="85"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -26799,7 +26561,7 @@
       <c r="U33" s="21"/>
     </row>
     <row r="34" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A34" s="85"/>
+      <c r="A34" s="83"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -26822,7 +26584,7 @@
       <c r="U34" s="21"/>
     </row>
     <row r="35" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A35" s="85"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -26847,7 +26609,7 @@
       <c r="X35" s="2"/>
     </row>
     <row r="36" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A36" s="85"/>
+      <c r="A36" s="83"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -26872,7 +26634,7 @@
       <c r="X36" s="2"/>
     </row>
     <row r="37" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A37" s="85"/>
+      <c r="A37" s="83"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -26899,7 +26661,7 @@
       <c r="Z37" s="20"/>
     </row>
     <row r="38" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A38" s="85"/>
+      <c r="A38" s="83"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
@@ -26926,7 +26688,7 @@
       <c r="Z38" s="21"/>
     </row>
     <row r="39" spans="1:26" ht="15" customHeight="1">
-      <c r="A39" s="85"/>
+      <c r="A39" s="83"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -26953,7 +26715,7 @@
       <c r="Z39" s="22"/>
     </row>
     <row r="40" spans="1:26" ht="15" customHeight="1">
-      <c r="A40" s="85"/>
+      <c r="A40" s="83"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
@@ -26980,7 +26742,7 @@
       <c r="Z40" s="22"/>
     </row>
     <row r="41" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A41" s="85"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -27007,7 +26769,7 @@
       <c r="Z41" s="22"/>
     </row>
     <row r="42" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A42" s="85"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
@@ -27034,7 +26796,7 @@
       <c r="Z42" s="22"/>
     </row>
     <row r="43" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A43" s="85"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -27061,7 +26823,7 @@
       <c r="Z43" s="22"/>
     </row>
     <row r="44" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A44" s="85"/>
+      <c r="A44" s="83"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
@@ -27084,7 +26846,7 @@
       <c r="U44" s="21"/>
     </row>
     <row r="45" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A45" s="85"/>
+      <c r="A45" s="83"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -27107,7 +26869,7 @@
       <c r="U45" s="21"/>
     </row>
     <row r="46" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A46" s="85"/>
+      <c r="A46" s="83"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
@@ -27130,7 +26892,7 @@
       <c r="U46" s="21"/>
     </row>
     <row r="47" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A47" s="85"/>
+      <c r="A47" s="83"/>
       <c r="B47" s="72"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -27153,7 +26915,7 @@
       <c r="U47" s="21"/>
     </row>
     <row r="48" spans="1:26" ht="18.75" customHeight="1">
-      <c r="A48" s="85"/>
+      <c r="A48" s="83"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
@@ -27176,7 +26938,7 @@
       <c r="U48" s="21"/>
     </row>
     <row r="49" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A49" s="85"/>
+      <c r="A49" s="83"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -27199,7 +26961,7 @@
       <c r="U49" s="21"/>
     </row>
     <row r="50" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A50" s="85"/>
+      <c r="A50" s="83"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
@@ -27222,7 +26984,7 @@
       <c r="U50" s="21"/>
     </row>
     <row r="51" spans="1:21" ht="15" customHeight="1">
-      <c r="A51" s="85"/>
+      <c r="A51" s="83"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -27245,7 +27007,7 @@
       <c r="U51" s="21"/>
     </row>
     <row r="52" spans="1:21" ht="15" customHeight="1">
-      <c r="A52" s="85"/>
+      <c r="A52" s="83"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
@@ -27268,7 +27030,7 @@
       <c r="U52" s="21"/>
     </row>
     <row r="53" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A53" s="85"/>
+      <c r="A53" s="83"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -27291,7 +27053,7 @@
       <c r="U53" s="21"/>
     </row>
     <row r="54" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A54" s="85"/>
+      <c r="A54" s="83"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -27314,7 +27076,7 @@
       <c r="U54" s="21"/>
     </row>
     <row r="55" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A55" s="85"/>
+      <c r="A55" s="83"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
@@ -27337,7 +27099,7 @@
       <c r="U55" s="21"/>
     </row>
     <row r="56" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A56" s="85"/>
+      <c r="A56" s="83"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
@@ -27360,7 +27122,7 @@
       <c r="U56" s="21"/>
     </row>
     <row r="57" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A57" s="85"/>
+      <c r="A57" s="83"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
@@ -27383,7 +27145,7 @@
       <c r="U57" s="21"/>
     </row>
     <row r="58" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A58" s="85"/>
+      <c r="A58" s="83"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
@@ -27406,7 +27168,7 @@
       <c r="U58" s="21"/>
     </row>
     <row r="59" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A59" s="85"/>
+      <c r="A59" s="83"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3"/>
@@ -27429,7 +27191,7 @@
       <c r="U59" s="21"/>
     </row>
     <row r="60" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A60" s="85"/>
+      <c r="A60" s="83"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3"/>
@@ -27452,7 +27214,7 @@
       <c r="U60" s="21"/>
     </row>
     <row r="61" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A61" s="85"/>
+      <c r="A61" s="83"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -27475,7 +27237,7 @@
       <c r="U61" s="21"/>
     </row>
     <row r="62" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A62" s="85"/>
+      <c r="A62" s="83"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
@@ -27498,7 +27260,7 @@
       <c r="U62" s="21"/>
     </row>
     <row r="63" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A63" s="85"/>
+      <c r="A63" s="83"/>
       <c r="B63" s="72"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
@@ -27521,7 +27283,7 @@
       <c r="U63" s="21"/>
     </row>
     <row r="64" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A64" s="85"/>
+      <c r="A64" s="83"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
@@ -27544,7 +27306,7 @@
       <c r="U64" s="21"/>
     </row>
     <row r="65" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A65" s="85"/>
+      <c r="A65" s="83"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
@@ -27567,7 +27329,7 @@
       <c r="U65" s="21"/>
     </row>
     <row r="66" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A66" s="85"/>
+      <c r="A66" s="83"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
@@ -27590,7 +27352,7 @@
       <c r="U66" s="21"/>
     </row>
     <row r="67" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A67" s="85"/>
+      <c r="A67" s="83"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
@@ -27613,7 +27375,7 @@
       <c r="U67" s="21"/>
     </row>
     <row r="68" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A68" s="85"/>
+      <c r="A68" s="83"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
@@ -27636,7 +27398,7 @@
       <c r="U68" s="21"/>
     </row>
     <row r="69" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A69" s="85"/>
+      <c r="A69" s="83"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3"/>
@@ -27659,7 +27421,7 @@
       <c r="U69" s="21"/>
     </row>
     <row r="70" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A70" s="85"/>
+      <c r="A70" s="83"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
       <c r="D70" s="3"/>
@@ -27682,7 +27444,7 @@
       <c r="U70" s="21"/>
     </row>
     <row r="71" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A71" s="85"/>
+      <c r="A71" s="83"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
@@ -27705,7 +27467,7 @@
       <c r="U71" s="21"/>
     </row>
     <row r="72" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A72" s="85"/>
+      <c r="A72" s="83"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3"/>
@@ -27728,7 +27490,7 @@
       <c r="U72" s="21"/>
     </row>
     <row r="73" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A73" s="85"/>
+      <c r="A73" s="83"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -27751,7 +27513,7 @@
       <c r="U73" s="21"/>
     </row>
     <row r="74" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A74" s="85"/>
+      <c r="A74" s="83"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
       <c r="D74" s="3"/>
@@ -27774,7 +27536,7 @@
       <c r="U74" s="21"/>
     </row>
     <row r="75" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A75" s="85"/>
+      <c r="A75" s="83"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3"/>
@@ -27797,7 +27559,7 @@
       <c r="U75" s="21"/>
     </row>
     <row r="76" spans="1:21" ht="15" customHeight="1">
-      <c r="A76" s="85"/>
+      <c r="A76" s="83"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3"/>
@@ -27820,7 +27582,7 @@
       <c r="U76" s="21"/>
     </row>
     <row r="77" spans="1:21" ht="15" customHeight="1">
-      <c r="A77" s="85"/>
+      <c r="A77" s="83"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3"/>
@@ -27843,7 +27605,7 @@
       <c r="U77" s="21"/>
     </row>
     <row r="78" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A78" s="85"/>
+      <c r="A78" s="83"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
       <c r="D78" s="3"/>
@@ -27866,7 +27628,7 @@
       <c r="U78" s="21"/>
     </row>
     <row r="79" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A79" s="85"/>
+      <c r="A79" s="83"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
       <c r="D79" s="3"/>
@@ -27889,24 +27651,24 @@
       <c r="U79" s="21"/>
     </row>
     <row r="80" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A80" s="85"/>
-      <c r="B80" s="104" t="s">
+      <c r="A80" s="83"/>
+      <c r="B80" s="86" t="s">
         <v>84</v>
       </c>
-      <c r="C80" s="104"/>
-      <c r="D80" s="104"/>
-      <c r="E80" s="104"/>
-      <c r="F80" s="104"/>
-      <c r="G80" s="104"/>
-      <c r="H80" s="104"/>
-      <c r="I80" s="104"/>
-      <c r="J80" s="104"/>
-      <c r="K80" s="104"/>
-      <c r="L80" s="104"/>
-      <c r="M80" s="104"/>
-      <c r="N80" s="104"/>
-      <c r="O80" s="104"/>
-      <c r="P80" s="104"/>
+      <c r="C80" s="86"/>
+      <c r="D80" s="86"/>
+      <c r="E80" s="86"/>
+      <c r="F80" s="86"/>
+      <c r="G80" s="86"/>
+      <c r="H80" s="86"/>
+      <c r="I80" s="86"/>
+      <c r="J80" s="86"/>
+      <c r="K80" s="86"/>
+      <c r="L80" s="86"/>
+      <c r="M80" s="86"/>
+      <c r="N80" s="86"/>
+      <c r="O80" s="86"/>
+      <c r="P80" s="86"/>
       <c r="Q80" s="3"/>
       <c r="R80" s="23"/>
       <c r="S80" s="21"/>
@@ -27914,22 +27676,22 @@
       <c r="U80" s="21"/>
     </row>
     <row r="81" spans="1:21" ht="57" customHeight="1">
-      <c r="A81" s="85"/>
-      <c r="B81" s="104"/>
-      <c r="C81" s="104"/>
-      <c r="D81" s="104"/>
-      <c r="E81" s="104"/>
-      <c r="F81" s="104"/>
-      <c r="G81" s="104"/>
-      <c r="H81" s="104"/>
-      <c r="I81" s="104"/>
-      <c r="J81" s="104"/>
-      <c r="K81" s="104"/>
-      <c r="L81" s="104"/>
-      <c r="M81" s="104"/>
-      <c r="N81" s="104"/>
-      <c r="O81" s="104"/>
-      <c r="P81" s="104"/>
+      <c r="A81" s="83"/>
+      <c r="B81" s="86"/>
+      <c r="C81" s="86"/>
+      <c r="D81" s="86"/>
+      <c r="E81" s="86"/>
+      <c r="F81" s="86"/>
+      <c r="G81" s="86"/>
+      <c r="H81" s="86"/>
+      <c r="I81" s="86"/>
+      <c r="J81" s="86"/>
+      <c r="K81" s="86"/>
+      <c r="L81" s="86"/>
+      <c r="M81" s="86"/>
+      <c r="N81" s="86"/>
+      <c r="O81" s="86"/>
+      <c r="P81" s="86"/>
       <c r="Q81" s="3"/>
       <c r="R81" s="23"/>
       <c r="S81" s="21"/>
@@ -27937,7 +27699,7 @@
       <c r="U81" s="21"/>
     </row>
     <row r="82" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A82" s="85"/>
+      <c r="A82" s="83"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
       <c r="D82" s="3"/>
@@ -27960,7 +27722,7 @@
       <c r="U82" s="21"/>
     </row>
     <row r="83" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A83" s="85"/>
+      <c r="A83" s="83"/>
       <c r="B83" s="72"/>
       <c r="C83" s="3"/>
       <c r="D83" s="3"/>
@@ -27983,7 +27745,7 @@
       <c r="U83" s="21"/>
     </row>
     <row r="84" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A84" s="85"/>
+      <c r="A84" s="83"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
       <c r="D84" s="3"/>
@@ -28006,7 +27768,7 @@
       <c r="U84" s="21"/>
     </row>
     <row r="85" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A85" s="85"/>
+      <c r="A85" s="83"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
       <c r="D85" s="3"/>
@@ -28029,7 +27791,7 @@
       <c r="U85" s="21"/>
     </row>
     <row r="86" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A86" s="85"/>
+      <c r="A86" s="83"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
       <c r="D86" s="3"/>
@@ -28052,7 +27814,7 @@
       <c r="U86" s="21"/>
     </row>
     <row r="87" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A87" s="85"/>
+      <c r="A87" s="83"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
       <c r="D87" s="3"/>
@@ -28075,7 +27837,7 @@
       <c r="U87" s="21"/>
     </row>
     <row r="88" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A88" s="85"/>
+      <c r="A88" s="83"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -28098,7 +27860,7 @@
       <c r="U88" s="21"/>
     </row>
     <row r="89" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A89" s="85"/>
+      <c r="A89" s="83"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -28121,7 +27883,7 @@
       <c r="U89" s="21"/>
     </row>
     <row r="90" spans="1:21" ht="15" customHeight="1">
-      <c r="A90" s="85"/>
+      <c r="A90" s="83"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
       <c r="D90" s="3"/>
@@ -28144,7 +27906,7 @@
       <c r="U90" s="21"/>
     </row>
     <row r="91" spans="1:21" ht="15" customHeight="1">
-      <c r="A91" s="85"/>
+      <c r="A91" s="83"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
       <c r="D91" s="3"/>
@@ -28167,7 +27929,7 @@
       <c r="U91" s="21"/>
     </row>
     <row r="92" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A92" s="85"/>
+      <c r="A92" s="83"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
       <c r="D92" s="3"/>
@@ -28190,7 +27952,7 @@
       <c r="U92" s="21"/>
     </row>
     <row r="93" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A93" s="85"/>
+      <c r="A93" s="83"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -28213,7 +27975,7 @@
       <c r="U93" s="21"/>
     </row>
     <row r="94" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A94" s="85"/>
+      <c r="A94" s="83"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
       <c r="D94" s="3"/>
@@ -28236,7 +27998,7 @@
       <c r="U94" s="21"/>
     </row>
     <row r="95" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A95" s="85"/>
+      <c r="A95" s="83"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
       <c r="D95" s="3"/>
@@ -28259,7 +28021,7 @@
       <c r="U95" s="21"/>
     </row>
     <row r="96" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A96" s="85"/>
+      <c r="A96" s="83"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
       <c r="D96" s="3"/>
@@ -28282,7 +28044,7 @@
       <c r="U96" s="21"/>
     </row>
     <row r="97" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A97" s="85"/>
+      <c r="A97" s="83"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
       <c r="D97" s="3"/>
@@ -28305,7 +28067,7 @@
       <c r="U97" s="21"/>
     </row>
     <row r="98" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A98" s="85"/>
+      <c r="A98" s="83"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
       <c r="D98" s="3"/>
@@ -28328,7 +28090,7 @@
       <c r="U98" s="21"/>
     </row>
     <row r="99" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A99" s="85"/>
+      <c r="A99" s="83"/>
       <c r="B99" s="72"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -28351,7 +28113,7 @@
       <c r="U99" s="21"/>
     </row>
     <row r="100" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A100" s="85"/>
+      <c r="A100" s="83"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -28374,7 +28136,7 @@
       <c r="U100" s="21"/>
     </row>
     <row r="101" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A101" s="85"/>
+      <c r="A101" s="83"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -28397,7 +28159,7 @@
       <c r="U101" s="21"/>
     </row>
     <row r="102" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A102" s="85"/>
+      <c r="A102" s="83"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
@@ -28420,7 +28182,7 @@
       <c r="U102" s="21"/>
     </row>
     <row r="103" spans="1:21" ht="15" customHeight="1">
-      <c r="A103" s="85"/>
+      <c r="A103" s="83"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -28443,7 +28205,7 @@
       <c r="U103" s="21"/>
     </row>
     <row r="104" spans="1:21" ht="15" customHeight="1">
-      <c r="A104" s="85"/>
+      <c r="A104" s="83"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -28466,7 +28228,7 @@
       <c r="U104" s="21"/>
     </row>
     <row r="105" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A105" s="85"/>
+      <c r="A105" s="83"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -28489,7 +28251,7 @@
       <c r="U105" s="21"/>
     </row>
     <row r="106" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A106" s="85"/>
+      <c r="A106" s="83"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -28512,7 +28274,7 @@
       <c r="U106" s="21"/>
     </row>
     <row r="107" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A107" s="85"/>
+      <c r="A107" s="83"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -28535,7 +28297,7 @@
       <c r="U107" s="21"/>
     </row>
     <row r="108" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A108" s="85"/>
+      <c r="A108" s="83"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
@@ -28558,7 +28320,7 @@
       <c r="U108" s="21"/>
     </row>
     <row r="109" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A109" s="85"/>
+      <c r="A109" s="83"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -28581,7 +28343,7 @@
       <c r="U109" s="21"/>
     </row>
     <row r="110" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A110" s="85"/>
+      <c r="A110" s="83"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -28604,7 +28366,7 @@
       <c r="U110" s="21"/>
     </row>
     <row r="111" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A111" s="85"/>
+      <c r="A111" s="83"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -28627,7 +28389,7 @@
       <c r="U111" s="21"/>
     </row>
     <row r="112" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A112" s="85"/>
+      <c r="A112" s="83"/>
       <c r="B112" s="3"/>
       <c r="C112" s="3"/>
       <c r="D112" s="3"/>
@@ -28650,7 +28412,7 @@
       <c r="U112" s="21"/>
     </row>
     <row r="113" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A113" s="85"/>
+      <c r="A113" s="83"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
@@ -28673,7 +28435,7 @@
       <c r="U113" s="21"/>
     </row>
     <row r="114" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A114" s="85"/>
+      <c r="A114" s="83"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
@@ -28696,7 +28458,7 @@
       <c r="U114" s="21"/>
     </row>
     <row r="115" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A115" s="85"/>
+      <c r="A115" s="83"/>
       <c r="B115" s="72"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -28719,7 +28481,7 @@
       <c r="U115" s="21"/>
     </row>
     <row r="116" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A116" s="85"/>
+      <c r="A116" s="83"/>
       <c r="B116" s="3"/>
       <c r="C116" s="3"/>
       <c r="D116" s="3"/>
@@ -28742,7 +28504,7 @@
       <c r="U116" s="21"/>
     </row>
     <row r="117" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A117" s="85"/>
+      <c r="A117" s="83"/>
       <c r="B117" s="3"/>
       <c r="C117" s="3"/>
       <c r="D117" s="3"/>
@@ -28765,7 +28527,7 @@
       <c r="U117" s="21"/>
     </row>
     <row r="118" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A118" s="85"/>
+      <c r="A118" s="83"/>
       <c r="B118" s="3"/>
       <c r="C118" s="3"/>
       <c r="D118" s="3"/>
@@ -28788,7 +28550,7 @@
       <c r="U118" s="21"/>
     </row>
     <row r="119" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A119" s="85"/>
+      <c r="A119" s="83"/>
       <c r="B119" s="3"/>
       <c r="C119" s="3"/>
       <c r="D119" s="3"/>
@@ -28811,7 +28573,7 @@
       <c r="U119" s="21"/>
     </row>
     <row r="120" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A120" s="85"/>
+      <c r="A120" s="83"/>
       <c r="B120" s="3"/>
       <c r="C120" s="3"/>
       <c r="D120" s="3"/>
@@ -28834,7 +28596,7 @@
       <c r="U120" s="21"/>
     </row>
     <row r="121" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A121" s="85"/>
+      <c r="A121" s="83"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
       <c r="D121" s="3"/>
@@ -28857,7 +28619,7 @@
       <c r="U121" s="21"/>
     </row>
     <row r="122" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A122" s="85"/>
+      <c r="A122" s="83"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
       <c r="D122" s="3"/>
@@ -28880,7 +28642,7 @@
       <c r="U122" s="21"/>
     </row>
     <row r="123" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A123" s="85"/>
+      <c r="A123" s="83"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
       <c r="D123" s="3"/>
@@ -28903,7 +28665,7 @@
       <c r="U123" s="21"/>
     </row>
     <row r="124" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A124" s="85"/>
+      <c r="A124" s="83"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
       <c r="D124" s="3"/>
@@ -28926,7 +28688,7 @@
       <c r="U124" s="21"/>
     </row>
     <row r="125" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A125" s="85"/>
+      <c r="A125" s="83"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
       <c r="D125" s="3"/>
@@ -28949,7 +28711,7 @@
       <c r="U125" s="21"/>
     </row>
     <row r="126" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A126" s="85"/>
+      <c r="A126" s="83"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
       <c r="D126" s="3"/>
@@ -28972,7 +28734,7 @@
       <c r="U126" s="21"/>
     </row>
     <row r="127" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A127" s="85"/>
+      <c r="A127" s="83"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
       <c r="D127" s="3"/>
@@ -28995,7 +28757,7 @@
       <c r="U127" s="21"/>
     </row>
     <row r="128" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A128" s="85"/>
+      <c r="A128" s="83"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
       <c r="D128" s="3"/>
@@ -29018,7 +28780,7 @@
       <c r="U128" s="21"/>
     </row>
     <row r="129" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A129" s="85"/>
+      <c r="A129" s="83"/>
       <c r="B129" s="3"/>
       <c r="C129" s="3"/>
       <c r="D129" s="3"/>
@@ -29041,7 +28803,7 @@
       <c r="U129" s="21"/>
     </row>
     <row r="130" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A130" s="85"/>
+      <c r="A130" s="83"/>
       <c r="B130" s="3"/>
       <c r="C130" s="3"/>
       <c r="D130" s="3"/>
@@ -29064,7 +28826,7 @@
       <c r="U130" s="21"/>
     </row>
     <row r="131" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A131" s="85"/>
+      <c r="A131" s="83"/>
       <c r="B131" s="3"/>
       <c r="C131" s="3"/>
       <c r="D131" s="3"/>
@@ -29087,24 +28849,24 @@
       <c r="U131" s="21"/>
     </row>
     <row r="132" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A132" s="85"/>
-      <c r="B132" s="103" t="s">
+      <c r="A132" s="83"/>
+      <c r="B132" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="C132" s="103"/>
-      <c r="D132" s="103"/>
-      <c r="E132" s="103"/>
-      <c r="F132" s="103"/>
-      <c r="G132" s="103"/>
-      <c r="H132" s="103"/>
-      <c r="I132" s="103"/>
-      <c r="J132" s="103"/>
-      <c r="K132" s="103"/>
-      <c r="L132" s="103"/>
-      <c r="M132" s="103"/>
-      <c r="N132" s="103"/>
-      <c r="O132" s="103"/>
-      <c r="P132" s="103"/>
+      <c r="C132" s="85"/>
+      <c r="D132" s="85"/>
+      <c r="E132" s="85"/>
+      <c r="F132" s="85"/>
+      <c r="G132" s="85"/>
+      <c r="H132" s="85"/>
+      <c r="I132" s="85"/>
+      <c r="J132" s="85"/>
+      <c r="K132" s="85"/>
+      <c r="L132" s="85"/>
+      <c r="M132" s="85"/>
+      <c r="N132" s="85"/>
+      <c r="O132" s="85"/>
+      <c r="P132" s="85"/>
       <c r="Q132" s="3"/>
       <c r="R132" s="23"/>
       <c r="S132" s="21"/>
@@ -29112,22 +28874,22 @@
       <c r="U132" s="21"/>
     </row>
     <row r="133" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A133" s="85"/>
-      <c r="B133" s="103"/>
-      <c r="C133" s="103"/>
-      <c r="D133" s="103"/>
-      <c r="E133" s="103"/>
-      <c r="F133" s="103"/>
-      <c r="G133" s="103"/>
-      <c r="H133" s="103"/>
-      <c r="I133" s="103"/>
-      <c r="J133" s="103"/>
-      <c r="K133" s="103"/>
-      <c r="L133" s="103"/>
-      <c r="M133" s="103"/>
-      <c r="N133" s="103"/>
-      <c r="O133" s="103"/>
-      <c r="P133" s="103"/>
+      <c r="A133" s="83"/>
+      <c r="B133" s="85"/>
+      <c r="C133" s="85"/>
+      <c r="D133" s="85"/>
+      <c r="E133" s="85"/>
+      <c r="F133" s="85"/>
+      <c r="G133" s="85"/>
+      <c r="H133" s="85"/>
+      <c r="I133" s="85"/>
+      <c r="J133" s="85"/>
+      <c r="K133" s="85"/>
+      <c r="L133" s="85"/>
+      <c r="M133" s="85"/>
+      <c r="N133" s="85"/>
+      <c r="O133" s="85"/>
+      <c r="P133" s="85"/>
       <c r="Q133" s="3"/>
       <c r="R133" s="23"/>
       <c r="S133" s="21"/>
@@ -29135,22 +28897,22 @@
       <c r="U133" s="21"/>
     </row>
     <row r="134" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A134" s="85"/>
-      <c r="B134" s="103"/>
-      <c r="C134" s="103"/>
-      <c r="D134" s="103"/>
-      <c r="E134" s="103"/>
-      <c r="F134" s="103"/>
-      <c r="G134" s="103"/>
-      <c r="H134" s="103"/>
-      <c r="I134" s="103"/>
-      <c r="J134" s="103"/>
-      <c r="K134" s="103"/>
-      <c r="L134" s="103"/>
-      <c r="M134" s="103"/>
-      <c r="N134" s="103"/>
-      <c r="O134" s="103"/>
-      <c r="P134" s="103"/>
+      <c r="A134" s="83"/>
+      <c r="B134" s="85"/>
+      <c r="C134" s="85"/>
+      <c r="D134" s="85"/>
+      <c r="E134" s="85"/>
+      <c r="F134" s="85"/>
+      <c r="G134" s="85"/>
+      <c r="H134" s="85"/>
+      <c r="I134" s="85"/>
+      <c r="J134" s="85"/>
+      <c r="K134" s="85"/>
+      <c r="L134" s="85"/>
+      <c r="M134" s="85"/>
+      <c r="N134" s="85"/>
+      <c r="O134" s="85"/>
+      <c r="P134" s="85"/>
       <c r="Q134" s="3"/>
       <c r="R134" s="23"/>
       <c r="S134" s="21"/>
@@ -29158,22 +28920,22 @@
       <c r="U134" s="21"/>
     </row>
     <row r="135" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A135" s="85"/>
-      <c r="B135" s="103"/>
-      <c r="C135" s="103"/>
-      <c r="D135" s="103"/>
-      <c r="E135" s="103"/>
-      <c r="F135" s="103"/>
-      <c r="G135" s="103"/>
-      <c r="H135" s="103"/>
-      <c r="I135" s="103"/>
-      <c r="J135" s="103"/>
-      <c r="K135" s="103"/>
-      <c r="L135" s="103"/>
-      <c r="M135" s="103"/>
-      <c r="N135" s="103"/>
-      <c r="O135" s="103"/>
-      <c r="P135" s="103"/>
+      <c r="A135" s="83"/>
+      <c r="B135" s="85"/>
+      <c r="C135" s="85"/>
+      <c r="D135" s="85"/>
+      <c r="E135" s="85"/>
+      <c r="F135" s="85"/>
+      <c r="G135" s="85"/>
+      <c r="H135" s="85"/>
+      <c r="I135" s="85"/>
+      <c r="J135" s="85"/>
+      <c r="K135" s="85"/>
+      <c r="L135" s="85"/>
+      <c r="M135" s="85"/>
+      <c r="N135" s="85"/>
+      <c r="O135" s="85"/>
+      <c r="P135" s="85"/>
       <c r="Q135" s="3"/>
       <c r="R135" s="23"/>
       <c r="S135" s="21"/>
@@ -29181,7 +28943,7 @@
       <c r="U135" s="21"/>
     </row>
     <row r="136" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A136" s="85"/>
+      <c r="A136" s="83"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
       <c r="D136" s="3"/>
@@ -29204,7 +28966,7 @@
       <c r="U136" s="21"/>
     </row>
     <row r="137" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A137" s="85"/>
+      <c r="A137" s="83"/>
       <c r="B137" s="72"/>
       <c r="C137" s="3"/>
       <c r="D137" s="3"/>
@@ -29227,7 +28989,7 @@
       <c r="U137" s="21"/>
     </row>
     <row r="138" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A138" s="85"/>
+      <c r="A138" s="83"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
       <c r="D138" s="3"/>
@@ -29250,7 +29012,7 @@
       <c r="U138" s="21"/>
     </row>
     <row r="139" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A139" s="85"/>
+      <c r="A139" s="83"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
       <c r="D139" s="3"/>
@@ -29273,7 +29035,7 @@
       <c r="U139" s="21"/>
     </row>
     <row r="140" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A140" s="85"/>
+      <c r="A140" s="83"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
       <c r="D140" s="3"/>
@@ -29296,7 +29058,7 @@
       <c r="U140" s="21"/>
     </row>
     <row r="141" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A141" s="85"/>
+      <c r="A141" s="83"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
       <c r="D141" s="3"/>
@@ -29319,7 +29081,7 @@
       <c r="U141" s="21"/>
     </row>
     <row r="142" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A142" s="85"/>
+      <c r="A142" s="83"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
       <c r="D142" s="3"/>
@@ -29342,7 +29104,7 @@
       <c r="U142" s="21"/>
     </row>
     <row r="143" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A143" s="85"/>
+      <c r="A143" s="83"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
       <c r="D143" s="3"/>
@@ -29365,7 +29127,7 @@
       <c r="U143" s="21"/>
     </row>
     <row r="144" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A144" s="85"/>
+      <c r="A144" s="83"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
       <c r="D144" s="3"/>
@@ -29388,7 +29150,7 @@
       <c r="U144" s="21"/>
     </row>
     <row r="145" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A145" s="85"/>
+      <c r="A145" s="83"/>
       <c r="B145" s="3"/>
       <c r="C145" s="3"/>
       <c r="D145" s="3"/>
@@ -29411,7 +29173,7 @@
       <c r="U145" s="21"/>
     </row>
     <row r="146" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A146" s="85"/>
+      <c r="A146" s="83"/>
       <c r="B146" s="3"/>
       <c r="C146" s="3"/>
       <c r="D146" s="3"/>
@@ -29434,7 +29196,7 @@
       <c r="U146" s="21"/>
     </row>
     <row r="147" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A147" s="85"/>
+      <c r="A147" s="83"/>
       <c r="B147" s="3"/>
       <c r="C147" s="3"/>
       <c r="D147" s="3"/>
@@ -29457,7 +29219,7 @@
       <c r="U147" s="21"/>
     </row>
     <row r="148" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A148" s="85"/>
+      <c r="A148" s="83"/>
       <c r="B148" s="3"/>
       <c r="C148" s="3"/>
       <c r="D148" s="3"/>
@@ -29480,7 +29242,7 @@
       <c r="U148" s="21"/>
     </row>
     <row r="149" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A149" s="85"/>
+      <c r="A149" s="83"/>
       <c r="B149" s="3"/>
       <c r="C149" s="3"/>
       <c r="D149" s="3"/>
@@ -29503,7 +29265,7 @@
       <c r="U149" s="21"/>
     </row>
     <row r="150" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A150" s="85"/>
+      <c r="A150" s="83"/>
       <c r="B150" s="3"/>
       <c r="C150" s="3"/>
       <c r="D150" s="3"/>
@@ -29526,7 +29288,7 @@
       <c r="U150" s="21"/>
     </row>
     <row r="151" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A151" s="85"/>
+      <c r="A151" s="83"/>
       <c r="B151" s="3"/>
       <c r="C151" s="3"/>
       <c r="D151" s="3"/>
@@ -29549,7 +29311,7 @@
       <c r="U151" s="21"/>
     </row>
     <row r="152" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A152" s="85"/>
+      <c r="A152" s="83"/>
       <c r="B152" s="3"/>
       <c r="C152" s="3"/>
       <c r="D152" s="3"/>
@@ -29572,7 +29334,7 @@
       <c r="U152" s="21"/>
     </row>
     <row r="153" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A153" s="85"/>
+      <c r="A153" s="83"/>
       <c r="B153" s="72"/>
       <c r="C153" s="3"/>
       <c r="D153" s="3"/>
@@ -29595,7 +29357,7 @@
       <c r="U153" s="21"/>
     </row>
     <row r="154" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A154" s="85"/>
+      <c r="A154" s="83"/>
       <c r="B154" s="3"/>
       <c r="C154" s="3"/>
       <c r="D154" s="3"/>
@@ -29618,7 +29380,7 @@
       <c r="U154" s="21"/>
     </row>
     <row r="155" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A155" s="85"/>
+      <c r="A155" s="83"/>
       <c r="B155" s="3"/>
       <c r="C155" s="3"/>
       <c r="D155" s="3"/>
@@ -29641,7 +29403,7 @@
       <c r="U155" s="21"/>
     </row>
     <row r="156" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A156" s="85"/>
+      <c r="A156" s="83"/>
       <c r="B156" s="3"/>
       <c r="C156" s="3"/>
       <c r="D156" s="3"/>
@@ -29664,7 +29426,7 @@
       <c r="U156" s="21"/>
     </row>
     <row r="157" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A157" s="85"/>
+      <c r="A157" s="83"/>
       <c r="B157" s="3"/>
       <c r="C157" s="3"/>
       <c r="D157" s="3"/>
@@ -29687,7 +29449,7 @@
       <c r="U157" s="21"/>
     </row>
     <row r="158" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A158" s="85"/>
+      <c r="A158" s="83"/>
       <c r="B158" s="3"/>
       <c r="C158" s="3"/>
       <c r="D158" s="3"/>
@@ -29710,7 +29472,7 @@
       <c r="U158" s="21"/>
     </row>
     <row r="159" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A159" s="85"/>
+      <c r="A159" s="83"/>
       <c r="B159" s="3"/>
       <c r="C159" s="3"/>
       <c r="D159" s="3"/>
@@ -29733,7 +29495,7 @@
       <c r="U159" s="21"/>
     </row>
     <row r="160" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A160" s="85"/>
+      <c r="A160" s="83"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>
       <c r="D160" s="3"/>
@@ -29756,7 +29518,7 @@
       <c r="U160" s="21"/>
     </row>
     <row r="161" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A161" s="85"/>
+      <c r="A161" s="83"/>
       <c r="B161" s="3"/>
       <c r="C161" s="3"/>
       <c r="D161" s="3"/>
@@ -29779,7 +29541,7 @@
       <c r="U161" s="21"/>
     </row>
     <row r="162" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A162" s="85"/>
+      <c r="A162" s="83"/>
       <c r="B162" s="3"/>
       <c r="C162" s="3"/>
       <c r="D162" s="3"/>
@@ -29802,7 +29564,7 @@
       <c r="U162" s="21"/>
     </row>
     <row r="163" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A163" s="85"/>
+      <c r="A163" s="83"/>
       <c r="B163" s="3"/>
       <c r="C163" s="3"/>
       <c r="D163" s="3"/>
@@ -29825,7 +29587,7 @@
       <c r="U163" s="21"/>
     </row>
     <row r="164" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A164" s="85"/>
+      <c r="A164" s="83"/>
       <c r="B164" s="3"/>
       <c r="C164" s="3"/>
       <c r="D164" s="3"/>
@@ -29848,7 +29610,7 @@
       <c r="U164" s="21"/>
     </row>
     <row r="165" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A165" s="85"/>
+      <c r="A165" s="83"/>
       <c r="B165" s="3"/>
       <c r="C165" s="3"/>
       <c r="D165" s="3"/>
@@ -29871,7 +29633,7 @@
       <c r="U165" s="21"/>
     </row>
     <row r="166" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A166" s="85"/>
+      <c r="A166" s="83"/>
       <c r="B166" s="3"/>
       <c r="C166" s="3"/>
       <c r="D166" s="3"/>
@@ -29894,7 +29656,7 @@
       <c r="U166" s="21"/>
     </row>
     <row r="167" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A167" s="85"/>
+      <c r="A167" s="83"/>
       <c r="B167" s="3"/>
       <c r="C167" s="3"/>
       <c r="D167" s="3"/>
@@ -29917,7 +29679,7 @@
       <c r="U167" s="21"/>
     </row>
     <row r="168" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A168" s="85"/>
+      <c r="A168" s="83"/>
       <c r="B168" s="3"/>
       <c r="C168" s="3"/>
       <c r="D168" s="3"/>
@@ -29940,7 +29702,7 @@
       <c r="U168" s="21"/>
     </row>
     <row r="169" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A169" s="85"/>
+      <c r="A169" s="83"/>
       <c r="B169" s="3"/>
       <c r="C169" s="3"/>
       <c r="D169" s="3"/>
@@ -29963,7 +29725,7 @@
       <c r="U169" s="21"/>
     </row>
     <row r="170" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A170" s="85"/>
+      <c r="A170" s="83"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
       <c r="D170" s="3"/>
@@ -29986,7 +29748,7 @@
       <c r="U170" s="21"/>
     </row>
     <row r="171" spans="1:23" ht="18.75" customHeight="1">
-      <c r="A171" s="84"/>
+      <c r="A171" s="82"/>
       <c r="B171" s="65"/>
       <c r="C171" s="65"/>
       <c r="D171" s="65"/>
@@ -30010,7 +29772,7 @@
       <c r="V171" s="25"/>
     </row>
     <row r="172" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A172" s="84"/>
+      <c r="A172" s="82"/>
       <c r="B172" s="25"/>
       <c r="C172" s="25"/>
       <c r="D172" s="25"/>
@@ -30035,7 +29797,7 @@
       <c r="W172" s="3"/>
     </row>
     <row r="173" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A173" s="84"/>
+      <c r="A173" s="82"/>
       <c r="B173" s="67"/>
       <c r="C173" s="68"/>
       <c r="D173" s="68"/>
@@ -30060,7 +29822,7 @@
       <c r="W173" s="3"/>
     </row>
     <row r="174" spans="1:23" ht="15" customHeight="1">
-      <c r="A174" s="84"/>
+      <c r="A174" s="82"/>
       <c r="B174" s="67"/>
       <c r="C174" s="68"/>
       <c r="D174" s="68"/>
@@ -30084,7 +29846,7 @@
       <c r="V174" s="25"/>
     </row>
     <row r="175" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A175" s="84"/>
+      <c r="A175" s="82"/>
       <c r="B175" s="67"/>
       <c r="C175" s="68"/>
       <c r="D175" s="68"/>
@@ -30108,7 +29870,7 @@
       <c r="V175" s="25"/>
     </row>
     <row r="176" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A176" s="84"/>
+      <c r="A176" s="82"/>
       <c r="B176" s="67"/>
       <c r="C176" s="68"/>
       <c r="D176" s="68"/>
@@ -30133,7 +29895,7 @@
       <c r="W176" s="3"/>
     </row>
     <row r="177" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A177" s="84"/>
+      <c r="A177" s="82"/>
       <c r="B177" s="25"/>
       <c r="C177" s="25"/>
       <c r="D177" s="25"/>
@@ -30158,7 +29920,7 @@
       <c r="W177" s="3"/>
     </row>
     <row r="178" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A178" s="84"/>
+      <c r="A178" s="82"/>
       <c r="B178" s="69"/>
       <c r="C178" s="69"/>
       <c r="D178" s="69"/>
@@ -30183,7 +29945,7 @@
       <c r="W178" s="3"/>
     </row>
     <row r="179" spans="1:23" s="4" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A179" s="84"/>
+      <c r="A179" s="82"/>
       <c r="B179" s="25"/>
       <c r="C179" s="25"/>
       <c r="D179" s="25"/>
@@ -31385,6 +31147,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B132:P135"/>
     <mergeCell ref="B80:P81"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="B5:D5"/>
@@ -31395,7 +31158,6 @@
     <mergeCell ref="S28:T29"/>
     <mergeCell ref="G28:K29"/>
     <mergeCell ref="J6:M7"/>
-    <mergeCell ref="B132:P135"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -31538,21 +31300,21 @@
     <row r="3" spans="2:22" ht="36" customHeight="1">
       <c r="B3" s="44"/>
       <c r="C3" s="45"/>
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="111" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
+      <c r="E3" s="111"/>
+      <c r="F3" s="111"/>
       <c r="G3" s="46"/>
-      <c r="H3" s="113" t="s">
+      <c r="H3" s="112" t="s">
         <v>64</v>
       </c>
-      <c r="I3" s="113"/>
-      <c r="J3" s="113"/>
-      <c r="K3" s="113"/>
-      <c r="L3" s="113"/>
-      <c r="M3" s="113"/>
-      <c r="N3" s="113"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
       <c r="O3" s="47"/>
       <c r="P3" s="45"/>
       <c r="Q3" s="45"/>
@@ -31589,85 +31351,85 @@
       <c r="B5" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="109" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="111"/>
-      <c r="G5" s="110" t="s">
+      <c r="E5" s="110"/>
+      <c r="G5" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="H5" s="111"/>
-      <c r="I5" s="110" t="s">
+      <c r="H5" s="110"/>
+      <c r="I5" s="109" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="111"/>
+      <c r="J5" s="110"/>
     </row>
     <row r="6" spans="2:22" ht="24.75" customHeight="1">
       <c r="B6" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="D6" s="105" t="s">
+      <c r="D6" s="104" t="s">
         <v>71</v>
       </c>
-      <c r="E6" s="106"/>
-      <c r="G6" s="105" t="s">
+      <c r="E6" s="105"/>
+      <c r="G6" s="104" t="s">
         <v>76</v>
       </c>
-      <c r="H6" s="106"/>
-      <c r="I6" s="105" t="s">
+      <c r="H6" s="105"/>
+      <c r="I6" s="104" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="106"/>
+      <c r="J6" s="105"/>
     </row>
     <row r="7" spans="2:22" ht="24.75" customHeight="1">
       <c r="B7" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="105" t="s">
+      <c r="G7" s="104" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="106"/>
-      <c r="I7" s="105" t="s">
+      <c r="H7" s="105"/>
+      <c r="I7" s="104" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="106"/>
+      <c r="J7" s="105"/>
     </row>
     <row r="8" spans="2:22" ht="24.75" customHeight="1">
       <c r="B8" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="105" t="s">
+      <c r="G8" s="104" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="106"/>
-      <c r="I8" s="105" t="s">
+      <c r="H8" s="105"/>
+      <c r="I8" s="104" t="s">
         <v>81</v>
       </c>
-      <c r="J8" s="106"/>
+      <c r="J8" s="105"/>
     </row>
     <row r="9" spans="2:22" ht="24.75" customHeight="1">
       <c r="B9" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="G9" s="105" t="s">
+      <c r="G9" s="104" t="s">
         <v>82</v>
       </c>
-      <c r="H9" s="106"/>
-      <c r="I9" s="105" t="s">
+      <c r="H9" s="105"/>
+      <c r="I9" s="104" t="s">
         <v>83</v>
       </c>
-      <c r="J9" s="106"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" spans="2:22" ht="24.75" customHeight="1">
       <c r="B10" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="G10" s="107" t="s">
+      <c r="G10" s="106" t="s">
         <v>73</v>
       </c>
-      <c r="H10" s="108"/>
-      <c r="I10" s="108"/>
-      <c r="J10" s="109"/>
+      <c r="H10" s="107"/>
+      <c r="I10" s="107"/>
+      <c r="J10" s="108"/>
     </row>
     <row r="11" spans="2:22" ht="24.75" customHeight="1">
       <c r="B11" s="49" t="s">

</xml_diff>